<commit_message>
Add Excel files and update all modules
</commit_message>
<xml_diff>
--- a/data/Implied_NOK_Defaults.xlsx
+++ b/data/Implied_NOK_Defaults.xlsx
@@ -675,8 +675,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010018D663DB1B96B8498A123F3887F55246" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48152895f98dae8470d04084b2345942">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9" xmlns:ns3="f6c676c0-61b9-4e26-a136-e78363c7067a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca4f743e3c406804796806514889b085" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010018D663DB1B96B8498A123F3887F55246" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="9fd2febd437389fd8a5d6c0b43c19e45">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9" xmlns:ns3="f6c676c0-61b9-4e26-a136-e78363c7067a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b6e6c383851e65736407ef4fd265b8f8" ns2:_="" ns3:_="">
     <xsd:import namespace="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9"/>
     <xsd:import namespace="f6c676c0-61b9-4e26-a136-e78363c7067a"/>
     <xsd:element name="properties">
@@ -724,7 +724,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="ba1ce1de-36b4-449a-bdef-96c47ebd2fcd" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkeringar" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="ba1ce1de-36b4-449a-bdef-96c47ebd2fcd" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -773,8 +773,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Innehållstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Rubrik"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -884,22 +884,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06D9DC94-8500-4902-8A8B-3172F89041AF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9"/>
-    <ds:schemaRef ds:uri="f6c676c0-61b9-4e26-a136-e78363c7067a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBE45617-68AA-4715-9B1D-7E329E8788EE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Uppdaterat charts.py med ny logik och fixat trace bugg
</commit_message>
<xml_diff>
--- a/data/Implied_NOK_Defaults.xlsx
+++ b/data/Implied_NOK_Defaults.xlsx
@@ -675,8 +675,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010018D663DB1B96B8498A123F3887F55246" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="9fd2febd437389fd8a5d6c0b43c19e45">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9" xmlns:ns3="f6c676c0-61b9-4e26-a136-e78363c7067a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b6e6c383851e65736407ef4fd265b8f8" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010018D663DB1B96B8498A123F3887F55246" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="19d493729cb5b1a8b93d4977cdad007b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9" xmlns:ns3="f6c676c0-61b9-4e26-a136-e78363c7067a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a726f3ab3b3527a96921f3312a9b266d" ns2:_="" ns3:_="">
     <xsd:import namespace="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9"/>
     <xsd:import namespace="f6c676c0-61b9-4e26-a136-e78363c7067a"/>
     <xsd:element name="properties">
@@ -884,7 +884,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBE45617-68AA-4715-9B1D-7E329E8788EE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B256E1-60A7-4FB5-817A-0829DB81A6E9}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Sparar mina lokala Excel-filer
</commit_message>
<xml_diff>
--- a/data/Implied_NOK_Defaults.xlsx
+++ b/data/Implied_NOK_Defaults.xlsx
@@ -675,8 +675,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010018D663DB1B96B8498A123F3887F55246" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="9fd2febd437389fd8a5d6c0b43c19e45">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9" xmlns:ns3="f6c676c0-61b9-4e26-a136-e78363c7067a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b6e6c383851e65736407ef4fd265b8f8" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x01010018D663DB1B96B8498A123F3887F55246" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="19d493729cb5b1a8b93d4977cdad007b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9" xmlns:ns3="f6c676c0-61b9-4e26-a136-e78363c7067a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a726f3ab3b3527a96921f3312a9b266d" ns2:_="" ns3:_="">
     <xsd:import namespace="d9c30b79-e6a1-4ed7-920c-5c2ba1b441f9"/>
     <xsd:import namespace="f6c676c0-61b9-4e26-a136-e78363c7067a"/>
     <xsd:element name="properties">
@@ -884,7 +884,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBE45617-68AA-4715-9B1D-7E329E8788EE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3055C27-AB47-4480-95C5-33C63CAD2515}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>